<commit_message>
ClassDiagram ,Progress status update
</commit_message>
<xml_diff>
--- a/PROGRESS/Unit1CA.xlsx
+++ b/PROGRESS/Unit1CA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8370" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="96">
   <si>
     <t>No.</t>
   </si>
@@ -332,6 +332,10 @@
   </si>
   <si>
     <t>StoreWindow</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>cancel</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -1012,9 +1016,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:K39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75"/>
@@ -1085,7 +1089,9 @@
       <c r="G3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="29"/>
+      <c r="H3" s="29">
+        <v>70</v>
+      </c>
     </row>
     <row r="4" spans="2:11">
       <c r="B4" s="15">
@@ -1105,7 +1111,9 @@
         <v>42083</v>
       </c>
       <c r="G4" s="16"/>
-      <c r="H4" s="29"/>
+      <c r="H4" s="29">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" spans="2:11">
       <c r="B5" s="15">
@@ -1127,7 +1135,9 @@
       <c r="G5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="29"/>
+      <c r="H5" s="29">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" spans="2:11">
       <c r="B6" s="15">
@@ -1147,7 +1157,9 @@
         <v>42083</v>
       </c>
       <c r="G6" s="16"/>
-      <c r="H6" s="29"/>
+      <c r="H6" s="29">
+        <v>70</v>
+      </c>
     </row>
     <row r="7" spans="2:11">
       <c r="B7" s="15">
@@ -1170,7 +1182,7 @@
         <v>13</v>
       </c>
       <c r="H7" s="29">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="2:11">
@@ -1194,7 +1206,7 @@
         <v>21</v>
       </c>
       <c r="H8" s="29">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="2:11">
@@ -1217,7 +1229,9 @@
       <c r="G9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="29"/>
+      <c r="H9" s="29">
+        <v>70</v>
+      </c>
     </row>
     <row r="10" spans="2:11">
       <c r="B10" s="15">
@@ -1239,7 +1253,9 @@
       <c r="G10" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="29"/>
+      <c r="H10" s="29">
+        <v>70</v>
+      </c>
     </row>
     <row r="11" spans="2:11">
       <c r="B11" s="15">
@@ -1261,7 +1277,9 @@
       <c r="G11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="29"/>
+      <c r="H11" s="29">
+        <v>70</v>
+      </c>
     </row>
     <row r="12" spans="2:11">
       <c r="B12" s="15">
@@ -1283,7 +1301,9 @@
       <c r="G12" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="29"/>
+      <c r="H12" s="29">
+        <v>70</v>
+      </c>
     </row>
     <row r="13" spans="2:11">
       <c r="B13" s="15">
@@ -1305,7 +1325,9 @@
       <c r="G13" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="29"/>
+      <c r="H13" s="29">
+        <v>70</v>
+      </c>
     </row>
     <row r="14" spans="2:11">
       <c r="B14" s="15">
@@ -1327,7 +1349,9 @@
       <c r="G14" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="29"/>
+      <c r="H14" s="29">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" spans="2:11">
       <c r="B15" s="15">
@@ -1349,7 +1373,9 @@
       <c r="G15" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="29"/>
+      <c r="H15" s="29">
+        <v>50</v>
+      </c>
     </row>
     <row r="16" spans="2:11">
       <c r="B16" s="15">
@@ -1372,7 +1398,7 @@
         <v>21</v>
       </c>
       <c r="H16" s="29">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="I16" s="39"/>
       <c r="J16" s="39"/>
@@ -1395,7 +1421,7 @@
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
       <c r="H17" s="35">
-        <v>20</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="2:8">
@@ -1416,7 +1442,9 @@
         <v>42090</v>
       </c>
       <c r="G18" s="24"/>
-      <c r="H18" s="36"/>
+      <c r="H18" s="36">
+        <v>70</v>
+      </c>
     </row>
     <row r="19" spans="2:8">
       <c r="B19" s="23">
@@ -1436,7 +1464,9 @@
         <v>42090</v>
       </c>
       <c r="G19" s="24"/>
-      <c r="H19" s="36"/>
+      <c r="H19" s="36">
+        <v>90</v>
+      </c>
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="23">
@@ -1450,13 +1480,15 @@
         <v>37</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F20" s="25">
         <v>42090</v>
       </c>
       <c r="G20" s="24"/>
-      <c r="H20" s="36"/>
+      <c r="H20" s="36">
+        <v>70</v>
+      </c>
     </row>
     <row r="21" spans="2:8">
       <c r="B21" s="23">
@@ -1568,7 +1600,9 @@
       <c r="G25" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="H25" s="36"/>
+      <c r="H25" s="36">
+        <v>70</v>
+      </c>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="23">
@@ -1590,7 +1624,9 @@
       <c r="G26" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="H26" s="36"/>
+      <c r="H26" s="36">
+        <v>70</v>
+      </c>
     </row>
     <row r="27" spans="2:8">
       <c r="B27" s="23">
@@ -1721,7 +1757,7 @@
       </c>
       <c r="G32" s="24"/>
       <c r="H32" s="36">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="2:11">
@@ -1782,7 +1818,9 @@
         <v>42090</v>
       </c>
       <c r="G35" s="24"/>
-      <c r="H35" s="36"/>
+      <c r="H35" s="36" t="s">
+        <v>95</v>
+      </c>
       <c r="I35" s="40"/>
       <c r="J35" s="39"/>
       <c r="K35" s="39"/>
@@ -1851,13 +1889,15 @@
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="17" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="F39" s="18">
         <v>42098</v>
       </c>
       <c r="G39" s="16"/>
-      <c r="H39" s="37"/>
+      <c r="H39" s="37">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="B2:H39"/>
@@ -2641,7 +2681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add CalcUtil to WBS
</commit_message>
<xml_diff>
--- a/PROGRESS/Unit1CA.xlsx
+++ b/PROGRESS/Unit1CA.xlsx
@@ -14,7 +14,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'coding WBS'!$B$2:$I$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Progress!$B$2:$H$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Progress!$B$2:$H$40</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="97">
   <si>
     <t>No.</t>
   </si>
@@ -336,6 +336,10 @@
   </si>
   <si>
     <t>cancel</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CalcUtil</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -673,6 +677,72 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1819275</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1073" name="流程图: 过程 37"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13201650" y="7219950"/>
+          <a:ext cx="1819275" cy="95250"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFD1BB"/>
+            </a:gs>
+            <a:gs pos="35001">
+              <a:srgbClr val="FFDDCF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFF2ED"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="F5913F"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1014,11 +1084,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:K39"/>
+  <dimension ref="B1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75"/>
@@ -1095,7 +1165,7 @@
     </row>
     <row r="4" spans="2:11">
       <c r="B4" s="15">
-        <f t="shared" ref="B4:B39" si="1">ROW()-2</f>
+        <f t="shared" ref="B4:B40" si="1">ROW()-2</f>
         <v>2</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -1744,20 +1814,20 @@
         <v>30</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="D32" s="24" t="s">
         <v>57</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="F32" s="25">
         <v>42090</v>
       </c>
       <c r="G32" s="24"/>
       <c r="H32" s="36">
-        <v>60</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="2:11">
@@ -1766,19 +1836,21 @@
         <v>31</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="17" t="s">
         <v>34</v>
       </c>
       <c r="F33" s="25">
         <v>42090</v>
       </c>
       <c r="G33" s="24"/>
-      <c r="H33" s="36"/>
+      <c r="H33" s="36">
+        <v>60</v>
+      </c>
     </row>
     <row r="34" spans="2:11">
       <c r="B34" s="23">
@@ -1786,13 +1858,13 @@
         <v>32</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="17" t="s">
-        <v>29</v>
+      <c r="E34" s="19" t="s">
+        <v>34</v>
       </c>
       <c r="F34" s="25">
         <v>42090</v>
@@ -1806,7 +1878,7 @@
         <v>33</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D35" s="24" t="s">
         <v>57</v>
@@ -1818,30 +1890,32 @@
         <v>42090</v>
       </c>
       <c r="G35" s="24"/>
-      <c r="H35" s="36" t="s">
+      <c r="H35" s="36"/>
+    </row>
+    <row r="36" spans="2:11">
+      <c r="B36" s="23">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="25">
+        <v>42090</v>
+      </c>
+      <c r="G36" s="24"/>
+      <c r="H36" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="I35" s="40"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-    </row>
-    <row r="36" spans="2:11">
-      <c r="B36" s="15">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="F36" s="18">
-        <v>42098</v>
-      </c>
-      <c r="G36" s="16"/>
-      <c r="H36" s="37"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="39"/>
     </row>
     <row r="37" spans="2:11">
       <c r="B37" s="15">
@@ -1849,7 +1923,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="17" t="s">
@@ -1867,7 +1941,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="17" t="s">
@@ -1885,26 +1959,45 @@
         <v>37</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="17" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="F39" s="18">
         <v>42098</v>
       </c>
       <c r="G39" s="16"/>
-      <c r="H39" s="37">
+      <c r="H39" s="37"/>
+    </row>
+    <row r="40" spans="2:11">
+      <c r="B40" s="15">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="16"/>
+      <c r="E40" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="18">
+        <v>42098</v>
+      </c>
+      <c r="G40" s="16"/>
+      <c r="H40" s="37">
         <v>100</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:H39"/>
+  <autoFilter ref="B2:H40"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>